<commit_message>
lab 2 aed done
</commit_message>
<xml_diff>
--- a/lab2_aed/lab2.xlsx
+++ b/lab2_aed/lab2.xlsx
@@ -8,35 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goncalo/studious-tribble/lab2_aed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3956E3-0069-B843-B038-932E98C579BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644EE284-AE10-9846-9960-A89FE4309AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2B21959B-35B5-49A9-925C-A901A10AF81D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{2B21959B-35B5-49A9-925C-A901A10AF81D}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Folha1!$B$19</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Folha1!$B$20:$B$34</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Folha1!$C$19</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Folha1!$C$20:$C$34</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Folha1!$D$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Folha1!$D$20:$D$34</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Folha1!$E$19</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Folha1!$E$20:$E$34</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Folha1!$F$19</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Folha1!$F$20:$F$34</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Folha1!$B$19</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Folha1!$B$20:$B$34</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Folha1!$C$19</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Folha1!$C$20:$C$34</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">Folha1!$D$19</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Folha1!$D$20:$D$34</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">Folha1!$E$19</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">Folha1!$E$20:$E$34</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">Folha1!$F$19</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">Folha1!$F$20:$F$34</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -220,11 +198,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2012,13 +1990,13 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
@@ -2037,26 +2015,26 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
@@ -2118,7 +2096,9 @@
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
@@ -2170,10 +2150,12 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>14</v>
+      </c>
       <c r="D4" s="1">
         <v>100</v>
       </c>
@@ -2228,7 +2210,9 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>165</v>
+      </c>
       <c r="D5" s="1">
         <v>1000</v>
       </c>
@@ -2283,7 +2267,9 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>1639</v>
+      </c>
       <c r="D6" s="1">
         <v>10000</v>
       </c>
@@ -2338,7 +2324,9 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>16256</v>
+      </c>
       <c r="D7" s="1">
         <v>100000</v>
       </c>
@@ -2617,7 +2605,7 @@
       <c r="D12" s="1">
         <v>200000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>167760</v>
       </c>
       <c r="F12" s="1">
@@ -2720,7 +2708,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="1"/>
@@ -2775,7 +2763,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="1"/>
@@ -2960,22 +2948,22 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
@@ -2984,16 +2972,16 @@
       <c r="C20" s="1">
         <v>100</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>33</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>32</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>46</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
@@ -3008,10 +2996,10 @@
       <c r="E21" s="1">
         <v>383</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>526</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
@@ -3026,10 +3014,10 @@
       <c r="E22" s="1">
         <v>4121</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>5461</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
@@ -3044,10 +3032,10 @@
       <c r="E23" s="1">
         <v>42542</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>54800</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
@@ -3062,10 +3050,10 @@
       <c r="E24" s="1">
         <v>431783</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>553085</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
@@ -3080,10 +3068,10 @@
       <c r="E25" s="1">
         <v>67</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <v>94</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
@@ -3098,10 +3086,10 @@
       <c r="E26" s="1">
         <v>772</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>1050</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
@@ -3116,10 +3104,10 @@
       <c r="E27" s="1">
         <v>8516</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>11088</v>
       </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
@@ -3134,10 +3122,10 @@
       <c r="E28" s="1">
         <v>85153</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="3">
         <v>110384</v>
       </c>
-      <c r="G28" s="4"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
@@ -3152,10 +3140,10 @@
       <c r="E29" s="1">
         <v>865847</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="3">
         <v>1106682</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
@@ -3170,10 +3158,10 @@
       <c r="E30" s="1">
         <v>189</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>258</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
@@ -3188,10 +3176,10 @@
       <c r="E31" s="1">
         <v>2076</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <v>2696</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
@@ -3206,10 +3194,10 @@
       <c r="E32" s="1">
         <v>21094</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F32" s="3">
         <v>27446</v>
       </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
@@ -3224,10 +3212,10 @@
       <c r="E33" s="1">
         <v>215308</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <v>276849</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
@@ -3242,10 +3230,10 @@
       <c r="E34" s="1">
         <v>2159282</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="3">
         <v>2765488</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>

</xml_diff>